<commit_message>
générateur de dataframe pour indicateur tri
</commit_message>
<xml_diff>
--- a/assets/Saisie-2023-INDICATEUR-DE-SUIVI-Ti.xlsx
+++ b/assets/Saisie-2023-INDICATEUR-DE-SUIVI-Ti.xlsx
@@ -4,15 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="2023-Ti-DF" sheetId="5" r:id="rId1"/>
-    <sheet name="2023-Ti-DRFD" sheetId="1" r:id="rId2"/>
-    <sheet name="2023-Ti-DIRE" sheetId="3" r:id="rId3"/>
-    <sheet name="2023-Ti-DAF" sheetId="2" r:id="rId4"/>
-    <sheet name="2023-Ti-DRH" sheetId="6" r:id="rId5"/>
-    <sheet name="2023-Ti-DRI" sheetId="4" r:id="rId6"/>
+    <sheet name="2023-DF-Tri" sheetId="5" r:id="rId1"/>
+    <sheet name="2023-DF-Annuel" sheetId="7" r:id="rId2"/>
+    <sheet name="2023-DRFD-Annuel" sheetId="1" r:id="rId3"/>
+    <sheet name="2023-DIRE-Tri" sheetId="3" r:id="rId4"/>
+    <sheet name="2023-DAF-Tri" sheetId="2" r:id="rId5"/>
+    <sheet name="2023-DAF-Annuel" sheetId="8" r:id="rId6"/>
+    <sheet name="2023-DRH-Annuel" sheetId="6" r:id="rId7"/>
+    <sheet name="2023-DRH-Tri" sheetId="9" r:id="rId8"/>
+    <sheet name="2023-DRI-Tri" sheetId="4" r:id="rId9"/>
+    <sheet name="2023-DRI-Annuel" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="125">
   <si>
     <t>Indicateur</t>
   </si>
@@ -935,10 +939,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:K12"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,38 +952,90 @@
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="19">
+        <v>600</v>
+      </c>
+      <c r="F2" s="19">
+        <v>600</v>
+      </c>
+      <c r="G2" s="19">
+        <v>600</v>
+      </c>
+      <c r="H2" s="19">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="19">
+        <v>55</v>
+      </c>
+      <c r="F3" s="19">
+        <v>55</v>
+      </c>
+      <c r="G3" s="19">
+        <v>55</v>
+      </c>
+      <c r="H3" s="19">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>21</v>
@@ -988,24 +1044,24 @@
         <v>41</v>
       </c>
       <c r="E4" s="19">
-        <v>600</v>
+        <v>50</v>
       </c>
       <c r="F4" s="19">
-        <v>600</v>
+        <v>50</v>
       </c>
       <c r="G4" s="19">
-        <v>600</v>
+        <v>50</v>
       </c>
       <c r="H4" s="19">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>21</v>
@@ -1014,24 +1070,24 @@
         <v>41</v>
       </c>
       <c r="E5" s="19">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F5" s="19">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G5" s="19">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H5" s="19">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>21</v>
@@ -1040,143 +1096,20 @@
         <v>41</v>
       </c>
       <c r="E6" s="19">
-        <v>50</v>
+        <f>SUM(E2:E5)</f>
+        <v>765</v>
       </c>
       <c r="F6" s="19">
-        <v>50</v>
+        <f t="shared" ref="F6:H6" si="0">SUM(F2:F5)</f>
+        <v>765</v>
       </c>
       <c r="G6" s="19">
-        <v>50</v>
-      </c>
-      <c r="H6" s="19">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="19">
-        <v>60</v>
-      </c>
-      <c r="F7" s="19">
-        <v>60</v>
-      </c>
-      <c r="G7" s="19">
-        <v>60</v>
-      </c>
-      <c r="H7" s="19">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="19">
-        <f>SUM(E4:E7)</f>
-        <v>765</v>
-      </c>
-      <c r="F8" s="19">
-        <f t="shared" ref="F8:H8" si="0">SUM(F4:F7)</f>
-        <v>765</v>
-      </c>
-      <c r="G8" s="19">
         <f t="shared" si="0"/>
         <v>765</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H6" s="19">
         <f t="shared" si="0"/>
         <v>765</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="21">
-        <v>1200</v>
-      </c>
-      <c r="F12" s="22">
-        <v>2200</v>
-      </c>
-      <c r="G12" s="19">
-        <v>2000</v>
-      </c>
-      <c r="H12" s="19">
-        <v>2400</v>
-      </c>
-      <c r="I12" s="19">
-        <v>1300</v>
-      </c>
-      <c r="J12" s="19">
-        <v>2500</v>
-      </c>
-      <c r="K12" s="19">
-        <f>SUM(E12:J12)</f>
-        <v>11600</v>
       </c>
     </row>
   </sheetData>
@@ -1185,12 +1118,147 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="8">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="21">
+        <v>1200</v>
+      </c>
+      <c r="F2" s="22">
+        <v>2200</v>
+      </c>
+      <c r="G2" s="19">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="19">
+        <v>2400</v>
+      </c>
+      <c r="I2" s="19">
+        <v>1300</v>
+      </c>
+      <c r="J2" s="19">
+        <v>2500</v>
+      </c>
+      <c r="K2" s="19">
+        <f>SUM(E2:J2)</f>
+        <v>11600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,16 +1388,25 @@
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="E4" s="5">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5">
+        <v>15</v>
+      </c>
+      <c r="J4" s="5">
+        <v>15</v>
+      </c>
+      <c r="K4" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1337,12 +1414,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,53 +1546,101 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="E2" s="19">
+        <v>200000</v>
+      </c>
+      <c r="F2" s="19">
+        <v>250000</v>
+      </c>
+      <c r="G2" s="19">
+        <v>200000</v>
+      </c>
+      <c r="H2" s="19">
+        <v>300000</v>
+      </c>
       <c r="I2" s="19">
         <f>SUM(E2:H2)</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
+        <v>950000</v>
+      </c>
+      <c r="J2" s="19">
+        <v>40000</v>
+      </c>
+      <c r="K2" s="19">
+        <v>40000</v>
+      </c>
+      <c r="L2" s="19">
+        <v>40000</v>
+      </c>
+      <c r="M2" s="19">
+        <v>40000</v>
+      </c>
       <c r="N2" s="19">
         <f>SUM(J2:M2)</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
+        <v>160000</v>
+      </c>
+      <c r="O2" s="19">
+        <v>150000</v>
+      </c>
+      <c r="P2" s="19">
+        <v>150000</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>150000</v>
+      </c>
+      <c r="R2" s="19">
+        <v>150000</v>
+      </c>
       <c r="S2" s="19">
         <f>SUM(O2:R2)</f>
-        <v>0</v>
-      </c>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
+        <v>600000</v>
+      </c>
+      <c r="T2" s="19">
+        <v>150000</v>
+      </c>
+      <c r="U2" s="19">
+        <v>150000</v>
+      </c>
+      <c r="V2" s="19">
+        <v>150000</v>
+      </c>
+      <c r="W2" s="19">
+        <v>150000</v>
+      </c>
       <c r="X2" s="19">
         <f>SUM(T2:W2)</f>
-        <v>0</v>
-      </c>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
+        <v>600000</v>
+      </c>
+      <c r="Y2" s="19">
+        <v>250000</v>
+      </c>
+      <c r="Z2" s="19">
+        <v>250000</v>
+      </c>
+      <c r="AA2" s="19">
+        <v>250000</v>
+      </c>
+      <c r="AB2" s="19">
+        <v>250000</v>
+      </c>
       <c r="AC2" s="19">
         <f>SUM(Y2:AB2)</f>
-        <v>0</v>
-      </c>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
+        <v>1000000</v>
+      </c>
+      <c r="AD2" s="19">
+        <v>200000</v>
+      </c>
+      <c r="AE2" s="19">
+        <v>250000</v>
+      </c>
+      <c r="AF2" s="19">
+        <v>200000</v>
+      </c>
+      <c r="AG2" s="19">
+        <v>250000</v>
+      </c>
       <c r="AH2" s="19">
         <f>SUM(AD2:AG2)</f>
-        <v>0</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1641,53 +1766,101 @@
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="19">
+        <v>16000</v>
+      </c>
+      <c r="F4" s="19">
+        <v>20000</v>
+      </c>
+      <c r="G4" s="19">
+        <v>16000</v>
+      </c>
+      <c r="H4" s="19">
+        <v>24000</v>
+      </c>
       <c r="I4" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
+        <v>76000</v>
+      </c>
+      <c r="J4" s="19">
+        <v>3500</v>
+      </c>
+      <c r="K4" s="19">
+        <v>3500</v>
+      </c>
+      <c r="L4" s="19">
+        <v>3500</v>
+      </c>
+      <c r="M4" s="19">
+        <v>3500</v>
+      </c>
       <c r="N4" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
+        <v>14000</v>
+      </c>
+      <c r="O4" s="19">
+        <v>12000</v>
+      </c>
+      <c r="P4" s="19">
+        <v>12000</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>12000</v>
+      </c>
+      <c r="R4" s="19">
+        <v>12000</v>
+      </c>
       <c r="S4" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
+        <v>48000</v>
+      </c>
+      <c r="T4" s="19">
+        <v>12000</v>
+      </c>
+      <c r="U4" s="19">
+        <v>12000</v>
+      </c>
+      <c r="V4" s="19">
+        <v>12000</v>
+      </c>
+      <c r="W4" s="19">
+        <v>12000</v>
+      </c>
       <c r="X4" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
+        <v>48000</v>
+      </c>
+      <c r="Y4" s="19">
+        <v>20000</v>
+      </c>
+      <c r="Z4" s="19">
+        <v>20000</v>
+      </c>
+      <c r="AA4" s="19">
+        <v>20000</v>
+      </c>
+      <c r="AB4" s="19">
+        <v>20000</v>
+      </c>
       <c r="AC4" s="19">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
+        <v>80000</v>
+      </c>
+      <c r="AD4" s="19">
+        <v>16000</v>
+      </c>
+      <c r="AE4" s="19">
+        <v>20000</v>
+      </c>
+      <c r="AF4" s="19">
+        <v>16000</v>
+      </c>
+      <c r="AG4" s="19">
+        <v>20000</v>
+      </c>
       <c r="AH4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>72000</v>
       </c>
     </row>
   </sheetData>
@@ -1696,12 +1869,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,100 +2112,100 @@
         <v>6</v>
       </c>
       <c r="E3" s="19">
-        <v>200000</v>
+        <v>70000</v>
       </c>
       <c r="F3" s="19">
-        <v>250000</v>
+        <v>80000</v>
       </c>
       <c r="G3" s="19">
-        <v>200000</v>
+        <v>70000</v>
       </c>
       <c r="H3" s="19">
-        <v>300000</v>
+        <v>100000</v>
       </c>
       <c r="I3" s="19">
         <f t="shared" ref="I3:I6" si="0">SUM(E3:H3)</f>
-        <v>950000</v>
+        <v>320000</v>
       </c>
       <c r="J3" s="19">
-        <v>40000</v>
+        <v>15000</v>
       </c>
       <c r="K3" s="19">
-        <v>40000</v>
+        <v>15000</v>
       </c>
       <c r="L3" s="19">
-        <v>40000</v>
+        <v>15000</v>
       </c>
       <c r="M3" s="19">
-        <v>40000</v>
+        <v>15000</v>
       </c>
       <c r="N3" s="19">
         <f t="shared" ref="N3:N6" si="1">SUM(J3:M3)</f>
-        <v>160000</v>
+        <v>60000</v>
       </c>
       <c r="O3" s="19">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="P3" s="19">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="Q3" s="19">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="R3" s="19">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="S3" s="19">
         <f t="shared" ref="S3:S6" si="2">SUM(O3:R3)</f>
-        <v>600000</v>
+        <v>200000</v>
       </c>
       <c r="T3" s="19">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="U3" s="19">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="V3" s="19">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="W3" s="19">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="X3" s="19">
         <f t="shared" ref="X3:X6" si="3">SUM(T3:W3)</f>
-        <v>600000</v>
+        <v>200000</v>
       </c>
       <c r="Y3" s="19">
-        <v>250000</v>
+        <v>80000</v>
       </c>
       <c r="Z3" s="19">
-        <v>250000</v>
+        <v>80000</v>
       </c>
       <c r="AA3" s="19">
-        <v>250000</v>
+        <v>80000</v>
       </c>
       <c r="AB3" s="19">
-        <v>250000</v>
+        <v>80000</v>
       </c>
       <c r="AC3" s="19">
         <f t="shared" ref="AC3:AC6" si="4">SUM(Y3:AB3)</f>
-        <v>1000000</v>
+        <v>320000</v>
       </c>
       <c r="AD3" s="19">
-        <v>200000</v>
+        <v>70000</v>
       </c>
       <c r="AE3" s="19">
-        <v>250000</v>
+        <v>80000</v>
       </c>
       <c r="AF3" s="19">
-        <v>200000</v>
+        <v>70000</v>
       </c>
       <c r="AG3" s="19">
-        <v>250000</v>
+        <v>80000</v>
       </c>
       <c r="AH3" s="19">
         <f t="shared" ref="AH3:AH6" si="5">SUM(AD3:AG3)</f>
-        <v>900000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2048,53 +2221,101 @@
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="19">
+        <v>130000</v>
+      </c>
+      <c r="F4" s="19">
+        <v>170000</v>
+      </c>
+      <c r="G4" s="19">
+        <v>130000</v>
+      </c>
+      <c r="H4" s="19">
+        <v>200000</v>
+      </c>
       <c r="I4" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
+        <v>630000</v>
+      </c>
+      <c r="J4" s="19">
+        <v>25000</v>
+      </c>
+      <c r="K4" s="19">
+        <v>25000</v>
+      </c>
+      <c r="L4" s="19">
+        <v>25000</v>
+      </c>
+      <c r="M4" s="19">
+        <v>25000</v>
+      </c>
       <c r="N4" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
+        <v>100000</v>
+      </c>
+      <c r="O4" s="19">
+        <v>100000</v>
+      </c>
+      <c r="P4" s="19">
+        <v>100000</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>100000</v>
+      </c>
+      <c r="R4" s="19">
+        <v>100000</v>
+      </c>
       <c r="S4" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
+        <v>400000</v>
+      </c>
+      <c r="T4" s="19">
+        <v>100000</v>
+      </c>
+      <c r="U4" s="19">
+        <v>100000</v>
+      </c>
+      <c r="V4" s="19">
+        <v>100000</v>
+      </c>
+      <c r="W4" s="19">
+        <v>100000</v>
+      </c>
       <c r="X4" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
+        <v>400000</v>
+      </c>
+      <c r="Y4" s="19">
+        <v>170000</v>
+      </c>
+      <c r="Z4" s="19">
+        <v>170000</v>
+      </c>
+      <c r="AA4" s="19">
+        <v>170000</v>
+      </c>
+      <c r="AB4" s="19">
+        <v>170000</v>
+      </c>
       <c r="AC4" s="19">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
+        <v>680000</v>
+      </c>
+      <c r="AD4" s="19">
+        <v>130000</v>
+      </c>
+      <c r="AE4" s="19">
+        <v>170000</v>
+      </c>
+      <c r="AF4" s="19">
+        <v>130000</v>
+      </c>
+      <c r="AG4" s="19">
+        <v>170000</v>
+      </c>
       <c r="AH4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2110,53 +2331,101 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="E5" s="19">
+        <v>160000</v>
+      </c>
+      <c r="F5" s="19">
+        <v>210000</v>
+      </c>
+      <c r="G5" s="19">
+        <v>165000</v>
+      </c>
+      <c r="H5" s="19">
+        <v>275000</v>
+      </c>
       <c r="I5" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
+        <v>810000</v>
+      </c>
+      <c r="J5" s="19">
+        <v>35000</v>
+      </c>
+      <c r="K5" s="19">
+        <v>35000</v>
+      </c>
+      <c r="L5" s="19">
+        <v>35000</v>
+      </c>
+      <c r="M5" s="19">
+        <v>35000</v>
+      </c>
       <c r="N5" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
+        <v>140000</v>
+      </c>
+      <c r="O5" s="19">
+        <v>135000</v>
+      </c>
+      <c r="P5" s="19">
+        <v>135000</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>135000</v>
+      </c>
+      <c r="R5" s="19">
+        <v>135000</v>
+      </c>
       <c r="S5" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
+        <v>540000</v>
+      </c>
+      <c r="T5" s="19">
+        <v>138000</v>
+      </c>
+      <c r="U5" s="19">
+        <v>138000</v>
+      </c>
+      <c r="V5" s="19">
+        <v>138000</v>
+      </c>
+      <c r="W5" s="19">
+        <v>138000</v>
+      </c>
       <c r="X5" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
+        <v>552000</v>
+      </c>
+      <c r="Y5" s="19">
+        <v>220000</v>
+      </c>
+      <c r="Z5" s="19">
+        <v>220000</v>
+      </c>
+      <c r="AA5" s="19">
+        <v>220000</v>
+      </c>
+      <c r="AB5" s="19">
+        <v>220000</v>
+      </c>
       <c r="AC5" s="19">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
+        <v>880000</v>
+      </c>
+      <c r="AD5" s="19">
+        <v>175000</v>
+      </c>
+      <c r="AE5" s="19">
+        <v>220000</v>
+      </c>
+      <c r="AF5" s="19">
+        <v>175000</v>
+      </c>
+      <c r="AG5" s="19">
+        <v>175000</v>
+      </c>
       <c r="AH5" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>745000</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2221,122 +2490,98 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" s="19">
-        <v>200000</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="P7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="R7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="S7" s="19">
-        <v>650000</v>
-      </c>
-      <c r="T7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="U7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="V7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="W7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="X7" s="19">
-        <v>650000</v>
-      </c>
-      <c r="Y7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC7" s="19">
-        <v>1100000</v>
-      </c>
-      <c r="AD7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH7" s="19">
-        <v>1000000</v>
-      </c>
-    </row>
+    <row r="7" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AG10" sqref="AG10"/>
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="F2" s="19">
+        <v>200000</v>
+      </c>
+      <c r="G2" s="19">
+        <v>650000</v>
+      </c>
+      <c r="H2" s="19">
+        <v>650000</v>
+      </c>
+      <c r="I2" s="19">
+        <v>1100000</v>
+      </c>
+      <c r="J2" s="19">
+        <v>1000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,7 +2592,7 @@
     <col min="29" max="29" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -2397,7 +2642,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="1"/>
@@ -2415,7 +2660,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -2466,7 +2711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -2516,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>70</v>
       </c>
@@ -2566,7 +2811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
@@ -2616,7 +2861,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
@@ -2664,203 +2909,6 @@
       </c>
       <c r="P7" s="12" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="P9" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="T9" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="X9" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB9" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="AC9" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD9" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE9" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF9" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="19">
-        <v>6</v>
-      </c>
-      <c r="F10" s="19">
-        <v>8</v>
-      </c>
-      <c r="G10" s="19">
-        <v>10</v>
-      </c>
-      <c r="H10" s="19">
-        <v>10</v>
-      </c>
-      <c r="I10" s="19">
-        <v>5</v>
-      </c>
-      <c r="J10" s="19">
-        <v>7</v>
-      </c>
-      <c r="K10" s="19">
-        <v>0</v>
-      </c>
-      <c r="L10" s="19">
-        <v>10</v>
-      </c>
-      <c r="M10" s="19">
-        <v>10</v>
-      </c>
-      <c r="N10" s="19">
-        <v>12</v>
-      </c>
-      <c r="O10" s="19">
-        <v>12</v>
-      </c>
-      <c r="P10" s="19">
-        <v>15</v>
-      </c>
-      <c r="Q10" s="19">
-        <v>10</v>
-      </c>
-      <c r="R10" s="19">
-        <v>10</v>
-      </c>
-      <c r="S10" s="19">
-        <v>12</v>
-      </c>
-      <c r="T10" s="19">
-        <v>15</v>
-      </c>
-      <c r="U10" s="19">
-        <v>12</v>
-      </c>
-      <c r="V10" s="19">
-        <v>14</v>
-      </c>
-      <c r="W10" s="19">
-        <v>16</v>
-      </c>
-      <c r="X10" s="19">
-        <v>20</v>
-      </c>
-      <c r="Y10" s="19">
-        <v>13</v>
-      </c>
-      <c r="Z10" s="19">
-        <v>15</v>
-      </c>
-      <c r="AA10" s="19">
-        <v>17</v>
-      </c>
-      <c r="AB10" s="19">
-        <v>20</v>
-      </c>
-      <c r="AC10" s="19">
-        <f>E10+Q10+U10+Y10+I10+M10</f>
-        <v>56</v>
-      </c>
-      <c r="AD10" s="19">
-        <f>F10+J10+N10+R10+V10+Z10</f>
-        <v>66</v>
-      </c>
-      <c r="AE10" s="19">
-        <f>G10+K10+O10+S10+W10+AB10</f>
-        <v>70</v>
-      </c>
-      <c r="AF10" s="19">
-        <f>H10+L10+P10+T10+X10+AB10</f>
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2869,12 +2917,224 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB1" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC1" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="19">
+        <v>6</v>
+      </c>
+      <c r="F2" s="19">
+        <v>8</v>
+      </c>
+      <c r="G2" s="19">
+        <v>10</v>
+      </c>
+      <c r="H2" s="19">
+        <v>10</v>
+      </c>
+      <c r="I2" s="19">
+        <v>5</v>
+      </c>
+      <c r="J2" s="19">
+        <v>7</v>
+      </c>
+      <c r="K2" s="19">
+        <v>0</v>
+      </c>
+      <c r="L2" s="19">
+        <v>10</v>
+      </c>
+      <c r="M2" s="19">
+        <v>10</v>
+      </c>
+      <c r="N2" s="19">
+        <v>12</v>
+      </c>
+      <c r="O2" s="19">
+        <v>12</v>
+      </c>
+      <c r="P2" s="19">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>10</v>
+      </c>
+      <c r="R2" s="19">
+        <v>10</v>
+      </c>
+      <c r="S2" s="19">
+        <v>12</v>
+      </c>
+      <c r="T2" s="19">
+        <v>15</v>
+      </c>
+      <c r="U2" s="19">
+        <v>12</v>
+      </c>
+      <c r="V2" s="19">
+        <v>14</v>
+      </c>
+      <c r="W2" s="19">
+        <v>16</v>
+      </c>
+      <c r="X2" s="19">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="19">
+        <v>13</v>
+      </c>
+      <c r="Z2" s="19">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="19">
+        <v>17</v>
+      </c>
+      <c r="AB2" s="19">
+        <v>20</v>
+      </c>
+      <c r="AC2" s="19">
+        <f>E2+Q2+U2+Y2+I2+M2</f>
+        <v>56</v>
+      </c>
+      <c r="AD2" s="19">
+        <f>F2+J2+N2+R2+V2+Z2</f>
+        <v>66</v>
+      </c>
+      <c r="AE2" s="19">
+        <f>G2+K2+O2+S2+W2+AB2</f>
+        <v>70</v>
+      </c>
+      <c r="AF2" s="19">
+        <f>H2+L2+P2+T2+X2+AB2</f>
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3041,40 +3301,6 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="8">
-        <v>150</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>